<commit_message>
Migrace results -> results_xlsx, vytvoření výsledků v csv
Hello
</commit_message>
<xml_diff>
--- a/results/seminarici_bez_seminare.xlsx
+++ b/results/seminarici_bez_seminare.xlsx
@@ -40,12 +40,12 @@
     <t>Regional geography of the Czech Republic</t>
   </si>
   <si>
+    <t>Programování A</t>
+  </si>
+  <si>
     <t>Počítačové modelování I</t>
   </si>
   <si>
-    <t>Programování A</t>
-  </si>
-  <si>
     <t>Identif. a hodn. ekosystémových služeb</t>
   </si>
   <si>
@@ -73,18 +73,18 @@
     <t>Softwarové inženýrství</t>
   </si>
   <si>
+    <t>Introduction to MATLAB</t>
+  </si>
+  <si>
     <t>Odborná prezentace</t>
   </si>
   <si>
-    <t>Introduction to MATLAB</t>
+    <t>EIS</t>
   </si>
   <si>
     <t>KEIS</t>
   </si>
   <si>
-    <t>EIS</t>
-  </si>
-  <si>
     <t>K521</t>
   </si>
   <si>
@@ -97,15 +97,15 @@
     <t>E101</t>
   </si>
   <si>
+    <t>K103</t>
+  </si>
+  <si>
+    <t>P107</t>
+  </si>
+  <si>
     <t>K107</t>
   </si>
   <si>
-    <t>P107</t>
-  </si>
-  <si>
-    <t>K103</t>
-  </si>
-  <si>
     <t>0153</t>
   </si>
   <si>
@@ -127,28 +127,28 @@
     <t>0158</t>
   </si>
   <si>
+    <t>KRSPP</t>
+  </si>
+  <si>
     <t>KSPP</t>
   </si>
   <si>
     <t>RSPP</t>
   </si>
   <si>
-    <t>KRSPP</t>
-  </si>
-  <si>
     <t>KSWI</t>
   </si>
   <si>
     <t>SWI</t>
   </si>
   <si>
+    <t>ITM</t>
+  </si>
+  <si>
+    <t>OPRE</t>
+  </si>
+  <si>
     <t>KOPRE</t>
-  </si>
-  <si>
-    <t>ITM</t>
-  </si>
-  <si>
-    <t>OPRE</t>
   </si>
 </sst>
 </file>
@@ -602,7 +602,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>28</v>
@@ -877,7 +877,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>44</v>

</xml_diff>